<commit_message>
variable names to match between data sets
</commit_message>
<xml_diff>
--- a/outcome_measurement/malaria/cod/match_dhis_names.xlsx
+++ b/outcome_measurement/malaria/cod/match_dhis_names.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13123" windowHeight="6103"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13120" windowHeight="6100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="379">
   <si>
     <t>A 1.8 Cas contacts parmi les nouveaux cas IST</t>
   </si>
@@ -762,9 +762,6 @@
     <t>ASAQstockOutDays_14yrsAndOlder</t>
   </si>
   <si>
-    <t>ASAQconsumed_14yrsAndOlder</t>
-  </si>
-  <si>
     <t>ASAQlost_14yrsAndOlder</t>
   </si>
   <si>
@@ -774,9 +771,6 @@
     <t>ASAQstockOutDays_1to5yrs</t>
   </si>
   <si>
-    <t>ASAQconsumed_1to5yrs</t>
-  </si>
-  <si>
     <t>ASAQlost_1to5yrs</t>
   </si>
   <si>
@@ -786,9 +780,6 @@
     <t>ASAQstockOutDays_2to11mos</t>
   </si>
   <si>
-    <t>ASAQconsumed_2to11mos</t>
-  </si>
-  <si>
     <t>ASAQlost_2to11mos</t>
   </si>
   <si>
@@ -798,9 +789,6 @@
     <t>ASAQstockOutDays_6to13yrs</t>
   </si>
   <si>
-    <t>ASAQconsumed_6to13yrs</t>
-  </si>
-  <si>
     <t>ASAQlost_6to13yrs</t>
   </si>
   <si>
@@ -810,9 +798,6 @@
     <t>ALstockOutDays_240mg40mg</t>
   </si>
   <si>
-    <t>Alconsumed_240mg40mg</t>
-  </si>
-  <si>
     <t>ALlost_240mg40mg</t>
   </si>
   <si>
@@ -822,15 +807,9 @@
     <t>ALstockOutDays_480mg80mg</t>
   </si>
   <si>
-    <t>ALconsumed_480mg80mg</t>
-  </si>
-  <si>
     <t>ALlost_480mg80mg</t>
   </si>
   <si>
-    <t>Alavailable_480mg80mg</t>
-  </si>
-  <si>
     <t>LLIN_stockOutDays</t>
   </si>
   <si>
@@ -871,6 +850,315 @@
   </si>
   <si>
     <t>indicator</t>
+  </si>
+  <si>
+    <t>ALavailable_480mg80mg</t>
+  </si>
+  <si>
+    <t>AL_40mg+240mg_available</t>
+  </si>
+  <si>
+    <t>AL_80mg+480mg_available</t>
+  </si>
+  <si>
+    <t>ASAQ_12to59mos_available</t>
+  </si>
+  <si>
+    <t>ASAQ_14yrsAndOlder_available</t>
+  </si>
+  <si>
+    <t>ASAQ_2to11mos_available</t>
+  </si>
+  <si>
+    <t>ASAQ_6to13yrs_available</t>
+  </si>
+  <si>
+    <t>ASAQ_inj_available</t>
+  </si>
+  <si>
+    <t>ASAQ_supp_200mg_available</t>
+  </si>
+  <si>
+    <t>ASAQ_supp_400mg_available</t>
+  </si>
+  <si>
+    <t>Quinine_inj_available</t>
+  </si>
+  <si>
+    <t>Quinine_tab_available</t>
+  </si>
+  <si>
+    <t>RHE_available</t>
+  </si>
+  <si>
+    <t>RHZ_available</t>
+  </si>
+  <si>
+    <t>RHZE_available</t>
+  </si>
+  <si>
+    <t>RH_150mg+75mg_available</t>
+  </si>
+  <si>
+    <t>RH_60mg+30mg_available</t>
+  </si>
+  <si>
+    <t>SP_available</t>
+  </si>
+  <si>
+    <t>AL_40mg+240mg_consumed</t>
+  </si>
+  <si>
+    <t>AL_80mg+480mg_consumed</t>
+  </si>
+  <si>
+    <t>ASAQ_12to59mos_consumed</t>
+  </si>
+  <si>
+    <t>ASAQ_14yrsAndOlder_consumed</t>
+  </si>
+  <si>
+    <t>ASAQ_2to11mos_consumed</t>
+  </si>
+  <si>
+    <t>ASAQ_6to13yrs_consumed</t>
+  </si>
+  <si>
+    <t>ASAQ_inj_consumed</t>
+  </si>
+  <si>
+    <t>ASAQ_supp_200mg_consumed</t>
+  </si>
+  <si>
+    <t>ASAQ_supp_400mg_consumed</t>
+  </si>
+  <si>
+    <t>Quinine_inj_consumed</t>
+  </si>
+  <si>
+    <t>Quinine_tab_consumed</t>
+  </si>
+  <si>
+    <t>RHE_consumed</t>
+  </si>
+  <si>
+    <t>RHZ_consumed</t>
+  </si>
+  <si>
+    <t>RHZE_consumed</t>
+  </si>
+  <si>
+    <t>RH_150mg+75mg_consumed</t>
+  </si>
+  <si>
+    <t>RH_60mg+30mg_consumed</t>
+  </si>
+  <si>
+    <t>SP_consumed</t>
+  </si>
+  <si>
+    <t>AL_40mg+240mg_lost</t>
+  </si>
+  <si>
+    <t>AL_80mg+480mg_lost</t>
+  </si>
+  <si>
+    <t>ASAQ_12to59mos_lost</t>
+  </si>
+  <si>
+    <t>ASAQ_14yrsAndOlder_lost</t>
+  </si>
+  <si>
+    <t>ASAQ_2to11mos_lost</t>
+  </si>
+  <si>
+    <t>ASAQ_6to13yrs_lost</t>
+  </si>
+  <si>
+    <t>ASAQ_inj_lost</t>
+  </si>
+  <si>
+    <t>ASAQ_supp_200mg_lost</t>
+  </si>
+  <si>
+    <t>ASAQ_supp_400mg_lost</t>
+  </si>
+  <si>
+    <t>Quinine_inj_lost</t>
+  </si>
+  <si>
+    <t>Quinine_tab_lost</t>
+  </si>
+  <si>
+    <t>RHE_lost</t>
+  </si>
+  <si>
+    <t>RHZ_lost</t>
+  </si>
+  <si>
+    <t>RHZE_lost</t>
+  </si>
+  <si>
+    <t>RH_150mg+75mg_lost</t>
+  </si>
+  <si>
+    <t>RH_60mg+30mg_lost</t>
+  </si>
+  <si>
+    <t>SP_lost</t>
+  </si>
+  <si>
+    <t>AL_40mg+240mg_received</t>
+  </si>
+  <si>
+    <t>AL_80mg+480mg_received</t>
+  </si>
+  <si>
+    <t>ASAQ_12to59mos_received</t>
+  </si>
+  <si>
+    <t>ASAQ_14yrsAndOlder_received</t>
+  </si>
+  <si>
+    <t>ASAQ_2to11mos_received</t>
+  </si>
+  <si>
+    <t>ASAQ_6to13yrs_received</t>
+  </si>
+  <si>
+    <t>ASAQ_inj_received</t>
+  </si>
+  <si>
+    <t>ASAQ_supp_200mg_received</t>
+  </si>
+  <si>
+    <t>ASAQ_supp_400mg_received</t>
+  </si>
+  <si>
+    <t>Quinine_inj_received</t>
+  </si>
+  <si>
+    <t>Quinine_tab_received</t>
+  </si>
+  <si>
+    <t>RHE_received</t>
+  </si>
+  <si>
+    <t>RHZ_received</t>
+  </si>
+  <si>
+    <t>RHZE_received</t>
+  </si>
+  <si>
+    <t>RH_150mg+75mg_received</t>
+  </si>
+  <si>
+    <t>RH_60mg+30mg_received</t>
+  </si>
+  <si>
+    <t>SP_received</t>
+  </si>
+  <si>
+    <t>ASAQused_14yrsAndOlder</t>
+  </si>
+  <si>
+    <t>ALused_240mg40mg</t>
+  </si>
+  <si>
+    <t>ASAQused_2to11mos</t>
+  </si>
+  <si>
+    <t>ASAQused_6to13yrs</t>
+  </si>
+  <si>
+    <t>ALused_480mg80mg</t>
+  </si>
+  <si>
+    <t>ASAQused_1to5yrs</t>
+  </si>
+  <si>
+    <t>QuinineConsumed_inj</t>
+  </si>
+  <si>
+    <t>QuinineConsumed_tab</t>
+  </si>
+  <si>
+    <t>RHavailable_60mg+30mg</t>
+  </si>
+  <si>
+    <t>RHavailable_150mg+75mg</t>
+  </si>
+  <si>
+    <t>RHconsumed_150mg+75mg</t>
+  </si>
+  <si>
+    <t>RHconsumed_60mg+30mg</t>
+  </si>
+  <si>
+    <t>QuinineAvailable_inj</t>
+  </si>
+  <si>
+    <t>QuinineAvailable_tab</t>
+  </si>
+  <si>
+    <t>QuinineLost_inj</t>
+  </si>
+  <si>
+    <t>ASconsumed_inj</t>
+  </si>
+  <si>
+    <t>ASlost_inj</t>
+  </si>
+  <si>
+    <t>RHlost_150mg+75mg</t>
+  </si>
+  <si>
+    <t>RHlost_60mg+30mg</t>
+  </si>
+  <si>
+    <t>ASavailable_inj</t>
+  </si>
+  <si>
+    <t>QuinineLost_tab</t>
+  </si>
+  <si>
+    <t>ALreceived_240mg40mg</t>
+  </si>
+  <si>
+    <t>ALreceived_480mg80mg</t>
+  </si>
+  <si>
+    <t>ASAQreceived_1to5yrs</t>
+  </si>
+  <si>
+    <t>ASAQreceived_14yrsAndOlder</t>
+  </si>
+  <si>
+    <t>ASAQreceived_2to11mos</t>
+  </si>
+  <si>
+    <t>ASAQreceived_6to13yrs</t>
+  </si>
+  <si>
+    <t>ASreceived_inj</t>
+  </si>
+  <si>
+    <t>ASreceived_supp200mg</t>
+  </si>
+  <si>
+    <t>ASreceived_supp400mg</t>
+  </si>
+  <si>
+    <t>RHreceived_150mg+75mg</t>
+  </si>
+  <si>
+    <t>RHreceived_60mg+30mg</t>
+  </si>
+  <si>
+    <t>QuinineReceived_inj</t>
+  </si>
+  <si>
+    <t>QuinineReceived_tab</t>
   </si>
 </sst>
 </file>
@@ -1204,31 +1492,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C215"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:C283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="B225" sqref="B225"/>
+    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="N271" sqref="N271"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.85" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="13.9" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.3828125" customWidth="1"/>
-    <col min="2" max="2" width="73.3046875" customWidth="1"/>
-    <col min="3" max="3" width="40.3828125" customWidth="1"/>
+    <col min="1" max="1" width="7.36328125" customWidth="1"/>
+    <col min="2" max="2" width="52.7265625" customWidth="1"/>
+    <col min="3" max="3" width="40.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>217</v>
       </c>
       <c r="B1" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C1" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1239,7 +1528,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1250,7 +1539,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1261,7 +1550,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1272,7 +1561,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1283,7 +1572,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1294,7 +1583,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1305,7 +1594,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1316,7 +1605,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1327,7 +1616,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1338,7 +1627,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1349,7 +1638,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1360,7 +1649,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1368,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1376,7 +1665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1384,7 +1673,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -1392,7 +1681,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1400,7 +1689,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1408,7 +1697,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1416,7 +1705,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1424,7 +1713,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -1432,7 +1721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -1440,7 +1729,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1448,7 +1737,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1456,7 +1745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -1464,7 +1753,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -1472,7 +1761,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1480,7 +1769,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1488,7 +1777,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -1496,7 +1785,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -1507,7 +1796,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -1518,7 +1807,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -1529,7 +1818,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -1540,7 +1829,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -1551,7 +1840,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -1562,7 +1851,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -1573,7 +1862,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -1581,7 +1870,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -1589,7 +1878,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -1597,7 +1886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -1605,7 +1894,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -1613,7 +1902,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -1621,7 +1910,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -1629,7 +1918,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -1637,7 +1926,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -1645,7 +1934,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -1653,7 +1942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1664,7 +1953,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1675,7 +1964,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1686,7 +1975,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -1697,7 +1986,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -1708,7 +1997,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -1719,7 +2008,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -1730,7 +2019,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -1741,7 +2030,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -1752,7 +2041,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>48</v>
       </c>
@@ -1760,10 +2049,10 @@
         <v>162</v>
       </c>
       <c r="C57" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>48</v>
       </c>
@@ -1771,10 +2060,10 @@
         <v>85</v>
       </c>
       <c r="C58" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -1782,10 +2071,10 @@
         <v>129</v>
       </c>
       <c r="C59" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>48</v>
       </c>
@@ -1793,10 +2082,10 @@
         <v>203</v>
       </c>
       <c r="C60" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -1804,10 +2093,10 @@
         <v>99</v>
       </c>
       <c r="C61" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -1815,10 +2104,10 @@
         <v>112</v>
       </c>
       <c r="C62" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>48</v>
       </c>
@@ -1826,10 +2115,10 @@
         <v>154</v>
       </c>
       <c r="C63" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>48</v>
       </c>
@@ -1837,10 +2126,10 @@
         <v>216</v>
       </c>
       <c r="C64" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>48</v>
       </c>
@@ -1848,10 +2137,10 @@
         <v>118</v>
       </c>
       <c r="C65" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>48</v>
       </c>
@@ -1859,10 +2148,10 @@
         <v>180</v>
       </c>
       <c r="C66" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>48</v>
       </c>
@@ -1870,10 +2159,10 @@
         <v>142</v>
       </c>
       <c r="C67" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>48</v>
       </c>
@@ -1881,10 +2170,10 @@
         <v>80</v>
       </c>
       <c r="C68" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>48</v>
       </c>
@@ -1892,10 +2181,10 @@
         <v>182</v>
       </c>
       <c r="C69" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>48</v>
       </c>
@@ -1903,10 +2192,10 @@
         <v>144</v>
       </c>
       <c r="C70" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>48</v>
       </c>
@@ -1914,10 +2203,10 @@
         <v>74</v>
       </c>
       <c r="C71" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>48</v>
       </c>
@@ -1925,7 +2214,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>48</v>
       </c>
@@ -1933,7 +2222,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>48</v>
       </c>
@@ -1941,7 +2230,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>48</v>
       </c>
@@ -1949,7 +2238,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>48</v>
       </c>
@@ -1957,7 +2246,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>48</v>
       </c>
@@ -1965,7 +2254,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>48</v>
       </c>
@@ -1973,7 +2262,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>48</v>
       </c>
@@ -1981,7 +2270,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>48</v>
       </c>
@@ -1989,7 +2278,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>48</v>
       </c>
@@ -1997,7 +2286,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>48</v>
       </c>
@@ -2005,7 +2294,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>48</v>
       </c>
@@ -2013,7 +2302,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>48</v>
       </c>
@@ -2021,10 +2310,10 @@
         <v>165</v>
       </c>
       <c r="C84" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -2032,10 +2321,10 @@
         <v>135</v>
       </c>
       <c r="C85" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -2043,10 +2332,10 @@
         <v>181</v>
       </c>
       <c r="C86" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>48</v>
       </c>
@@ -2054,10 +2343,10 @@
         <v>128</v>
       </c>
       <c r="C87" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>48</v>
       </c>
@@ -2065,10 +2354,10 @@
         <v>170</v>
       </c>
       <c r="C88" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>48</v>
       </c>
@@ -2076,10 +2365,10 @@
         <v>116</v>
       </c>
       <c r="C89" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>48</v>
       </c>
@@ -2087,10 +2376,10 @@
         <v>102</v>
       </c>
       <c r="C90" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>48</v>
       </c>
@@ -2098,10 +2387,10 @@
         <v>184</v>
       </c>
       <c r="C91" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>48</v>
       </c>
@@ -2109,10 +2398,10 @@
         <v>68</v>
       </c>
       <c r="C92" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>48</v>
       </c>
@@ -2120,10 +2409,10 @@
         <v>101</v>
       </c>
       <c r="C93" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>48</v>
       </c>
@@ -2131,10 +2420,10 @@
         <v>215</v>
       </c>
       <c r="C94" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>48</v>
       </c>
@@ -2142,10 +2431,10 @@
         <v>53</v>
       </c>
       <c r="C95" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -2153,7 +2442,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>48</v>
       </c>
@@ -2161,7 +2450,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>48</v>
       </c>
@@ -2169,7 +2458,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>48</v>
       </c>
@@ -2177,7 +2466,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>48</v>
       </c>
@@ -2185,7 +2474,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>48</v>
       </c>
@@ -2193,7 +2482,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>48</v>
       </c>
@@ -2201,7 +2490,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>48</v>
       </c>
@@ -2209,7 +2498,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>48</v>
       </c>
@@ -2217,7 +2506,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>48</v>
       </c>
@@ -2225,7 +2514,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>48</v>
       </c>
@@ -2233,7 +2522,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>48</v>
       </c>
@@ -2241,7 +2530,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>48</v>
       </c>
@@ -2249,7 +2538,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>48</v>
       </c>
@@ -2257,7 +2546,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>48</v>
       </c>
@@ -2265,7 +2554,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="111" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>48</v>
       </c>
@@ -2273,7 +2562,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="112" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>48</v>
       </c>
@@ -2281,7 +2570,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>48</v>
       </c>
@@ -2289,7 +2578,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>48</v>
       </c>
@@ -2297,7 +2586,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>48</v>
       </c>
@@ -2305,7 +2594,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>48</v>
       </c>
@@ -2313,7 +2602,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>48</v>
       </c>
@@ -2321,7 +2610,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>48</v>
       </c>
@@ -2329,7 +2618,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>48</v>
       </c>
@@ -2337,7 +2626,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>48</v>
       </c>
@@ -2345,7 +2634,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="121" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>48</v>
       </c>
@@ -2353,7 +2642,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>48</v>
       </c>
@@ -2361,7 +2650,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>48</v>
       </c>
@@ -2369,7 +2658,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>48</v>
       </c>
@@ -2377,7 +2666,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>48</v>
       </c>
@@ -2385,7 +2674,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>48</v>
       </c>
@@ -2393,7 +2682,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>48</v>
       </c>
@@ -2401,7 +2690,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>48</v>
       </c>
@@ -2409,10 +2698,10 @@
         <v>176</v>
       </c>
       <c r="C128" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>48</v>
       </c>
@@ -2420,10 +2709,10 @@
         <v>55</v>
       </c>
       <c r="C129" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>48</v>
       </c>
@@ -2431,10 +2720,10 @@
         <v>98</v>
       </c>
       <c r="C130" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>48</v>
       </c>
@@ -2442,10 +2731,10 @@
         <v>189</v>
       </c>
       <c r="C131" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>48</v>
       </c>
@@ -2453,10 +2742,10 @@
         <v>122</v>
       </c>
       <c r="C132" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>48</v>
       </c>
@@ -2464,10 +2753,10 @@
         <v>143</v>
       </c>
       <c r="C133" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>48</v>
       </c>
@@ -2475,10 +2764,10 @@
         <v>109</v>
       </c>
       <c r="C134" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>48</v>
       </c>
@@ -2486,10 +2775,10 @@
         <v>73</v>
       </c>
       <c r="C135" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>51</v>
       </c>
@@ -2497,7 +2786,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>51</v>
       </c>
@@ -2505,7 +2794,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>51</v>
       </c>
@@ -2513,7 +2802,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>51</v>
       </c>
@@ -2521,7 +2810,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>51</v>
       </c>
@@ -2529,7 +2818,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>51</v>
       </c>
@@ -2537,7 +2826,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>51</v>
       </c>
@@ -2545,7 +2834,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>51</v>
       </c>
@@ -2553,7 +2842,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>51</v>
       </c>
@@ -2561,7 +2850,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>51</v>
       </c>
@@ -2569,7 +2858,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>51</v>
       </c>
@@ -2577,7 +2866,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>51</v>
       </c>
@@ -2585,7 +2874,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>51</v>
       </c>
@@ -2593,7 +2882,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>51</v>
       </c>
@@ -2601,7 +2890,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>51</v>
       </c>
@@ -2609,7 +2898,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>51</v>
       </c>
@@ -2617,7 +2906,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>51</v>
       </c>
@@ -2625,7 +2914,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>51</v>
       </c>
@@ -2633,7 +2922,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>51</v>
       </c>
@@ -2641,7 +2930,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>51</v>
       </c>
@@ -2649,7 +2938,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>51</v>
       </c>
@@ -2657,7 +2946,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>51</v>
       </c>
@@ -2665,7 +2954,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>51</v>
       </c>
@@ -2673,7 +2962,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>51</v>
       </c>
@@ -2681,7 +2970,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>51</v>
       </c>
@@ -2689,7 +2978,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>51</v>
       </c>
@@ -2697,7 +2986,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>51</v>
       </c>
@@ -2705,7 +2994,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>51</v>
       </c>
@@ -2713,7 +3002,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>51</v>
       </c>
@@ -2721,7 +3010,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>51</v>
       </c>
@@ -2729,7 +3018,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>51</v>
       </c>
@@ -2737,7 +3026,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>51</v>
       </c>
@@ -2745,7 +3034,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>51</v>
       </c>
@@ -2753,7 +3042,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>51</v>
       </c>
@@ -2761,7 +3050,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>51</v>
       </c>
@@ -2769,7 +3058,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>51</v>
       </c>
@@ -2777,7 +3066,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>51</v>
       </c>
@@ -2785,7 +3074,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>51</v>
       </c>
@@ -2793,7 +3082,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>51</v>
       </c>
@@ -2801,7 +3090,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>51</v>
       </c>
@@ -2809,7 +3098,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>51</v>
       </c>
@@ -2817,7 +3106,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>51</v>
       </c>
@@ -2825,7 +3114,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>51</v>
       </c>
@@ -2833,7 +3122,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>51</v>
       </c>
@@ -2841,7 +3130,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>51</v>
       </c>
@@ -2849,7 +3138,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>51</v>
       </c>
@@ -2857,7 +3146,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>51</v>
       </c>
@@ -2865,7 +3154,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>51</v>
       </c>
@@ -2873,7 +3162,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>51</v>
       </c>
@@ -2881,7 +3170,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>51</v>
       </c>
@@ -2889,7 +3178,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>51</v>
       </c>
@@ -2897,7 +3186,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>51</v>
       </c>
@@ -2905,7 +3194,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>51</v>
       </c>
@@ -2913,7 +3202,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>51</v>
       </c>
@@ -2921,7 +3210,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>51</v>
       </c>
@@ -2929,7 +3218,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>51</v>
       </c>
@@ -2937,7 +3226,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>51</v>
       </c>
@@ -2945,7 +3234,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>51</v>
       </c>
@@ -2953,7 +3242,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>51</v>
       </c>
@@ -2961,7 +3250,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>51</v>
       </c>
@@ -2969,7 +3258,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>51</v>
       </c>
@@ -2977,7 +3266,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>51</v>
       </c>
@@ -2985,7 +3274,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>51</v>
       </c>
@@ -2993,7 +3282,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>51</v>
       </c>
@@ -3001,7 +3290,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>51</v>
       </c>
@@ -3009,7 +3298,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>51</v>
       </c>
@@ -3017,7 +3306,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>51</v>
       </c>
@@ -3025,7 +3314,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>51</v>
       </c>
@@ -3033,7 +3322,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>51</v>
       </c>
@@ -3041,7 +3330,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>51</v>
       </c>
@@ -3049,7 +3338,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>51</v>
       </c>
@@ -3057,7 +3346,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>51</v>
       </c>
@@ -3065,7 +3354,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:2" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>51</v>
       </c>
@@ -3073,7 +3362,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>51</v>
       </c>
@@ -3081,7 +3370,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="210" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>51</v>
       </c>
@@ -3089,7 +3378,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>51</v>
       </c>
@@ -3097,7 +3386,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>51</v>
       </c>
@@ -3105,7 +3394,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>51</v>
       </c>
@@ -3113,7 +3402,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>51</v>
       </c>
@@ -3121,7 +3410,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="13.85" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:3" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>51</v>
       </c>
@@ -3129,13 +3418,767 @@
         <v>75</v>
       </c>
     </row>
+    <row r="216" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
+        <v>48</v>
+      </c>
+      <c r="B216" t="s">
+        <v>277</v>
+      </c>
+      <c r="C216" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>48</v>
+      </c>
+      <c r="B217" t="s">
+        <v>278</v>
+      </c>
+      <c r="C217" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>48</v>
+      </c>
+      <c r="B218" t="s">
+        <v>279</v>
+      </c>
+      <c r="C218" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>48</v>
+      </c>
+      <c r="B219" t="s">
+        <v>280</v>
+      </c>
+      <c r="C219" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>48</v>
+      </c>
+      <c r="B220" t="s">
+        <v>281</v>
+      </c>
+      <c r="C220" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>48</v>
+      </c>
+      <c r="B221" t="s">
+        <v>282</v>
+      </c>
+      <c r="C221" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
+        <v>51</v>
+      </c>
+      <c r="B222" t="s">
+        <v>283</v>
+      </c>
+      <c r="C222" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
+        <v>48</v>
+      </c>
+      <c r="B223" t="s">
+        <v>284</v>
+      </c>
+      <c r="C223" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
+        <v>48</v>
+      </c>
+      <c r="B224" t="s">
+        <v>285</v>
+      </c>
+      <c r="C224" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>51</v>
+      </c>
+      <c r="B225" t="s">
+        <v>286</v>
+      </c>
+      <c r="C225" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>51</v>
+      </c>
+      <c r="B226" t="s">
+        <v>287</v>
+      </c>
+      <c r="C226" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
+        <v>48</v>
+      </c>
+      <c r="B227" t="s">
+        <v>288</v>
+      </c>
+      <c r="C227" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
+        <v>48</v>
+      </c>
+      <c r="B228" t="s">
+        <v>289</v>
+      </c>
+      <c r="C228" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
+        <v>48</v>
+      </c>
+      <c r="B229" t="s">
+        <v>290</v>
+      </c>
+      <c r="C229" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A230" t="s">
+        <v>48</v>
+      </c>
+      <c r="B230" t="s">
+        <v>291</v>
+      </c>
+      <c r="C230" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
+        <v>48</v>
+      </c>
+      <c r="B231" t="s">
+        <v>292</v>
+      </c>
+      <c r="C231" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
+        <v>48</v>
+      </c>
+      <c r="B232" t="s">
+        <v>293</v>
+      </c>
+      <c r="C232" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A233" t="s">
+        <v>48</v>
+      </c>
+      <c r="B233" t="s">
+        <v>294</v>
+      </c>
+      <c r="C233" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A234" t="s">
+        <v>48</v>
+      </c>
+      <c r="B234" t="s">
+        <v>295</v>
+      </c>
+      <c r="C234" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A235" t="s">
+        <v>48</v>
+      </c>
+      <c r="B235" t="s">
+        <v>296</v>
+      </c>
+      <c r="C235" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A236" t="s">
+        <v>48</v>
+      </c>
+      <c r="B236" t="s">
+        <v>297</v>
+      </c>
+      <c r="C236" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A237" t="s">
+        <v>48</v>
+      </c>
+      <c r="B237" t="s">
+        <v>298</v>
+      </c>
+      <c r="C237" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A238" t="s">
+        <v>48</v>
+      </c>
+      <c r="B238" t="s">
+        <v>299</v>
+      </c>
+      <c r="C238" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A239" t="s">
+        <v>51</v>
+      </c>
+      <c r="B239" t="s">
+        <v>300</v>
+      </c>
+      <c r="C239" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A240" t="s">
+        <v>48</v>
+      </c>
+      <c r="B240" t="s">
+        <v>301</v>
+      </c>
+      <c r="C240" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A241" t="s">
+        <v>48</v>
+      </c>
+      <c r="B241" t="s">
+        <v>302</v>
+      </c>
+      <c r="C241" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A242" t="s">
+        <v>51</v>
+      </c>
+      <c r="B242" t="s">
+        <v>303</v>
+      </c>
+      <c r="C242" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A243" t="s">
+        <v>51</v>
+      </c>
+      <c r="B243" t="s">
+        <v>304</v>
+      </c>
+      <c r="C243" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A244" t="s">
+        <v>48</v>
+      </c>
+      <c r="B244" t="s">
+        <v>305</v>
+      </c>
+      <c r="C244" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A245" t="s">
+        <v>48</v>
+      </c>
+      <c r="B245" t="s">
+        <v>306</v>
+      </c>
+      <c r="C245" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A246" t="s">
+        <v>48</v>
+      </c>
+      <c r="B246" t="s">
+        <v>307</v>
+      </c>
+      <c r="C246" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A247" t="s">
+        <v>48</v>
+      </c>
+      <c r="B247" t="s">
+        <v>308</v>
+      </c>
+      <c r="C247" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A248" t="s">
+        <v>48</v>
+      </c>
+      <c r="B248" t="s">
+        <v>309</v>
+      </c>
+      <c r="C248" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A249" t="s">
+        <v>48</v>
+      </c>
+      <c r="B249" t="s">
+        <v>310</v>
+      </c>
+      <c r="C249" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A250" t="s">
+        <v>48</v>
+      </c>
+      <c r="B250" t="s">
+        <v>311</v>
+      </c>
+      <c r="C250" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A251" t="s">
+        <v>48</v>
+      </c>
+      <c r="B251" t="s">
+        <v>312</v>
+      </c>
+      <c r="C251" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A252" t="s">
+        <v>48</v>
+      </c>
+      <c r="B252" t="s">
+        <v>313</v>
+      </c>
+      <c r="C252" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A253" t="s">
+        <v>48</v>
+      </c>
+      <c r="B253" t="s">
+        <v>314</v>
+      </c>
+      <c r="C253" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A254" t="s">
+        <v>48</v>
+      </c>
+      <c r="B254" t="s">
+        <v>315</v>
+      </c>
+      <c r="C254" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A255" t="s">
+        <v>48</v>
+      </c>
+      <c r="B255" t="s">
+        <v>316</v>
+      </c>
+      <c r="C255" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A256" t="s">
+        <v>51</v>
+      </c>
+      <c r="B256" t="s">
+        <v>317</v>
+      </c>
+      <c r="C256" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A257" t="s">
+        <v>48</v>
+      </c>
+      <c r="B257" t="s">
+        <v>318</v>
+      </c>
+      <c r="C257" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A258" t="s">
+        <v>48</v>
+      </c>
+      <c r="B258" t="s">
+        <v>319</v>
+      </c>
+      <c r="C258" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A259" t="s">
+        <v>51</v>
+      </c>
+      <c r="B259" t="s">
+        <v>320</v>
+      </c>
+      <c r="C259" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A260" t="s">
+        <v>51</v>
+      </c>
+      <c r="B260" t="s">
+        <v>321</v>
+      </c>
+      <c r="C260" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A261" t="s">
+        <v>48</v>
+      </c>
+      <c r="B261" t="s">
+        <v>322</v>
+      </c>
+      <c r="C261" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A262" t="s">
+        <v>48</v>
+      </c>
+      <c r="B262" t="s">
+        <v>323</v>
+      </c>
+      <c r="C262" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A263" t="s">
+        <v>48</v>
+      </c>
+      <c r="B263" t="s">
+        <v>324</v>
+      </c>
+      <c r="C263" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A264" t="s">
+        <v>48</v>
+      </c>
+      <c r="B264" t="s">
+        <v>325</v>
+      </c>
+      <c r="C264" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A265" t="s">
+        <v>48</v>
+      </c>
+      <c r="B265" t="s">
+        <v>326</v>
+      </c>
+      <c r="C265" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A266" t="s">
+        <v>48</v>
+      </c>
+      <c r="B266" t="s">
+        <v>327</v>
+      </c>
+      <c r="C266" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A267" t="s">
+        <v>48</v>
+      </c>
+      <c r="B267" t="s">
+        <v>328</v>
+      </c>
+      <c r="C267" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A268" t="s">
+        <v>48</v>
+      </c>
+      <c r="B268" t="s">
+        <v>329</v>
+      </c>
+      <c r="C268" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A269" t="s">
+        <v>48</v>
+      </c>
+      <c r="B269" t="s">
+        <v>330</v>
+      </c>
+      <c r="C269" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A270" t="s">
+        <v>48</v>
+      </c>
+      <c r="B270" t="s">
+        <v>331</v>
+      </c>
+      <c r="C270" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A271" t="s">
+        <v>48</v>
+      </c>
+      <c r="B271" t="s">
+        <v>332</v>
+      </c>
+      <c r="C271" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A272" t="s">
+        <v>48</v>
+      </c>
+      <c r="B272" t="s">
+        <v>333</v>
+      </c>
+      <c r="C272" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A273" t="s">
+        <v>51</v>
+      </c>
+      <c r="B273" t="s">
+        <v>334</v>
+      </c>
+      <c r="C273" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A274" t="s">
+        <v>48</v>
+      </c>
+      <c r="B274" t="s">
+        <v>335</v>
+      </c>
+      <c r="C274" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A275" t="s">
+        <v>48</v>
+      </c>
+      <c r="B275" t="s">
+        <v>336</v>
+      </c>
+      <c r="C275" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A276" t="s">
+        <v>51</v>
+      </c>
+      <c r="B276" t="s">
+        <v>337</v>
+      </c>
+      <c r="C276" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A277" t="s">
+        <v>51</v>
+      </c>
+      <c r="B277" t="s">
+        <v>338</v>
+      </c>
+      <c r="C277" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A278" t="s">
+        <v>48</v>
+      </c>
+      <c r="B278" t="s">
+        <v>339</v>
+      </c>
+      <c r="C278" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A279" t="s">
+        <v>48</v>
+      </c>
+      <c r="B279" t="s">
+        <v>340</v>
+      </c>
+      <c r="C279" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A280" t="s">
+        <v>48</v>
+      </c>
+      <c r="B280" t="s">
+        <v>341</v>
+      </c>
+      <c r="C280" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A281" t="s">
+        <v>48</v>
+      </c>
+      <c r="B281" t="s">
+        <v>342</v>
+      </c>
+      <c r="C281" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A282" t="s">
+        <v>48</v>
+      </c>
+      <c r="B282" t="s">
+        <v>343</v>
+      </c>
+      <c r="C282" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A283" t="s">
+        <v>48</v>
+      </c>
+      <c r="B283" t="s">
+        <v>344</v>
+      </c>
+      <c r="C283" t="s">
+        <v>344</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:C215"/>
+  <autoFilter ref="A2:C215">
+    <filterColumn colId="2">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A1:C215">
     <sortCondition ref="A1:A215"/>
     <sortCondition ref="B1:B215"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>